<commit_message>
color coding markers; add tooltip
</commit_message>
<xml_diff>
--- a/kings/data/heros.xlsx
+++ b/kings/data/heros.xlsx
@@ -1131,9 +1131,6 @@
     <t>长城，魔族，大唐，都护府，沙漠，绿洲，西域</t>
   </si>
   <si>
-    <t>Time_ZH</t>
-  </si>
-  <si>
     <t>一说春秋战国卫国朝歌（河南淇县）人；一说是战国魏国邺地（河北临漳）人；一说陈国郸城（河南郸城县）人</t>
   </si>
   <si>
@@ -2719,12 +2716,6 @@
     <t>河南南阳人</t>
   </si>
   <si>
-    <t>曾隐居于湖北隆中。</t>
-  </si>
-  <si>
-    <t>陈塘关（河南西峡?）总兵之子。</t>
-  </si>
-  <si>
     <t>西汉</t>
   </si>
   <si>
@@ -2848,9 +2839,6 @@
     <t>无盐邑（山东东平）人</t>
   </si>
   <si>
-    <t>涿县人</t>
-  </si>
-  <si>
     <t>燕人</t>
   </si>
   <si>
@@ -2894,6 +2882,18 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>于易水辞别太子丹出发刺秦王</t>
+  </si>
+  <si>
+    <t>曾大闹东海（==）</t>
+  </si>
+  <si>
+    <t>曾隐居于湖北隆中</t>
   </si>
 </sst>
 </file>
@@ -2980,8 +2980,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3028,7 +3038,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3048,6 +3058,11 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3067,6 +3082,11 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -3104,7 +3124,7 @@
     <tableColumn id="5" name="avatar"/>
     <tableColumn id="12" name="fictious"/>
     <tableColumn id="6" name="note"/>
-    <tableColumn id="14" name="Time_ZH"/>
+    <tableColumn id="14" name="time"/>
     <tableColumn id="7" name="location"/>
     <tableColumn id="16" name="lat"/>
     <tableColumn id="18" name="lng"/>
@@ -3442,10 +3462,10 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3485,22 +3505,22 @@
         <v>361</v>
       </c>
       <c r="H1" t="s">
-        <v>370</v>
+        <v>585</v>
       </c>
       <c r="I1" t="s">
         <v>360</v>
       </c>
       <c r="J1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="K1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="L1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="M1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N1" t="s">
         <v>363</v>
@@ -3523,16 +3543,16 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>364</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J2">
         <v>37.814689399999999</v>
@@ -3541,10 +3561,10 @@
         <v>115.6592857</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="N2" t="s">
         <v>366</v>
@@ -3567,16 +3587,16 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>367</v>
       </c>
       <c r="H3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J3">
         <v>39.7309567</v>
@@ -3585,10 +3605,10 @@
         <v>97.974348000000006</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3608,16 +3628,16 @@
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>368</v>
       </c>
       <c r="H4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J4">
         <v>39.7309567</v>
@@ -3626,10 +3646,10 @@
         <v>97.974348000000006</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3649,16 +3669,16 @@
         <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>369</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J5">
         <v>41.720764000000003</v>
@@ -3667,10 +3687,10 @@
         <v>82.940991299999993</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3690,16 +3710,16 @@
         <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>372</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J6">
         <v>35.654178600000002</v>
@@ -3708,10 +3728,10 @@
         <v>114.0090587</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -3731,16 +3751,16 @@
         <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J7">
         <v>30.619397800000002</v>
@@ -3749,10 +3769,10 @@
         <v>119.8203345</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -3772,16 +3792,16 @@
         <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J8">
         <v>30.424098300000001</v>
@@ -3790,10 +3810,10 @@
         <v>112.1543722</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -3813,16 +3833,16 @@
         <v>44</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>376</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J9">
         <v>30.764525200000001</v>
@@ -3831,10 +3851,10 @@
         <v>116.2269744</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -3854,16 +3874,16 @@
         <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J10">
         <v>32.997202700000003</v>
@@ -3872,10 +3892,10 @@
         <v>112.4134935</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -3895,16 +3915,16 @@
         <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>530</v>
+        <v>588</v>
       </c>
       <c r="J11">
         <v>32.482154600000001</v>
@@ -3913,10 +3933,10 @@
         <v>111.7061947</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -3936,28 +3956,28 @@
         <v>59</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>380</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>531</v>
+        <v>587</v>
       </c>
       <c r="J12">
-        <v>33.444897400000002</v>
+        <v>30.272139899999999</v>
       </c>
       <c r="K12">
-        <v>111.1359035</v>
+        <v>125.7833835</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -3977,16 +3997,16 @@
         <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="J13">
         <v>31.836822999999999</v>
@@ -3995,10 +4015,10 @@
         <v>104.6394653</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -4018,16 +4038,16 @@
         <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="J14">
         <v>37.863274199999999</v>
@@ -4036,13 +4056,13 @@
         <v>112.47253259999999</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N14" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -4062,16 +4082,16 @@
         <v>74</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J15">
         <v>37.990831999999997</v>
@@ -4080,10 +4100,10 @@
         <v>23.703319799999999</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -4103,16 +4123,16 @@
         <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J16">
         <v>32.042321200000004</v>
@@ -4121,10 +4141,10 @@
         <v>105.09346619999999</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -4144,16 +4164,16 @@
         <v>84</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="J17">
         <v>48.741565999999999</v>
@@ -4162,13 +4182,13 @@
         <v>109.8304</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="N17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -4188,16 +4208,16 @@
         <v>89</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J18">
         <v>34.019576999999998</v>
@@ -4206,10 +4226,10 @@
         <v>108.6126233</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -4229,16 +4249,16 @@
         <v>94</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="J19">
         <v>33.320701</v>
@@ -4247,10 +4267,10 @@
         <v>117.5538603</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -4270,16 +4290,16 @@
         <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>365</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J20">
         <v>37.927478999999998</v>
@@ -4288,10 +4308,10 @@
         <v>102.56646859999999</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -4311,16 +4331,16 @@
         <v>104</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J21">
         <v>39.479145099999997</v>
@@ -4329,10 +4349,10 @@
         <v>115.8559377</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -4352,16 +4372,16 @@
         <v>109</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J22">
         <v>39.479145099999997</v>
@@ -4370,10 +4390,10 @@
         <v>115.85593780000001</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -4393,16 +4413,16 @@
         <v>114</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G23" t="s">
+        <v>391</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>393</v>
-      </c>
       <c r="I23" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="J23">
         <v>34.4129407</v>
@@ -4411,10 +4431,10 @@
         <v>115.50749690000001</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -4434,16 +4454,16 @@
         <v>119</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J24">
         <v>42.9263865</v>
@@ -4452,10 +4472,10 @@
         <v>89.516201300000006</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -4475,16 +4495,16 @@
         <v>124</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="J25">
         <v>34.6666861</v>
@@ -4493,10 +4513,10 @@
         <v>119.210003</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -4516,16 +4536,16 @@
         <v>129</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J26">
         <v>51.528308000000003</v>
@@ -4534,10 +4554,10 @@
         <v>-0.38178050000000002</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -4557,16 +4577,16 @@
         <v>134</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="I27" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="J27">
         <v>35.245809199999997</v>
@@ -4575,10 +4595,10 @@
         <v>135.5488953</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -4598,16 +4618,16 @@
         <v>139</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="J28">
         <v>43.415644299999997</v>
@@ -4616,10 +4636,10 @@
         <v>140.33260379999999</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -4639,16 +4659,16 @@
         <v>144</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H29" t="s">
+        <v>471</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="J29">
         <v>35.669107400000001</v>
@@ -4657,10 +4677,10 @@
         <v>139.60129470000001</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -4680,16 +4700,16 @@
         <v>149</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>403</v>
-      </c>
       <c r="I30" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J30">
         <v>33.906655700000002</v>
@@ -4698,10 +4718,10 @@
         <v>112.73247000000001</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -4721,16 +4741,16 @@
         <v>154</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G31" t="s">
+        <v>403</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="I31" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="J31">
         <v>34.117657999999999</v>
@@ -4739,10 +4759,10 @@
         <v>115.7900763</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -4762,16 +4782,16 @@
         <v>159</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J32">
         <v>36.607000800000002</v>
@@ -4780,10 +4800,10 @@
         <v>114.3429464</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -4803,16 +4823,16 @@
         <v>164</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J33">
         <v>47.891628799999999</v>
@@ -4821,10 +4841,10 @@
         <v>106.83183219999999</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -4844,16 +4864,16 @@
         <v>169</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="J34">
         <v>33.632400799999999</v>
@@ -4862,10 +4882,10 @@
         <v>118.68467579999999</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -4885,16 +4905,16 @@
         <v>174</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J35">
         <v>34.698483199999998</v>
@@ -4903,10 +4923,10 @@
         <v>116.5851059</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -4926,16 +4946,16 @@
         <v>179</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="J36">
         <v>34.366756199999998</v>
@@ -4944,10 +4964,10 @@
         <v>107.0864843</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -4967,16 +4987,16 @@
         <v>184</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J37">
         <v>34.4129407</v>
@@ -4985,10 +5005,10 @@
         <v>115.50749690000001</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -5008,16 +5028,16 @@
         <v>189</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="I38" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="J38">
         <v>35.973823500000002</v>
@@ -5026,10 +5046,10 @@
         <v>116.2166884</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -5049,16 +5069,16 @@
         <v>194</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J39">
         <v>51.528308000000003</v>
@@ -5067,10 +5087,10 @@
         <v>-0.38178050000000002</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -5090,16 +5110,16 @@
         <v>199</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G40" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="J40">
         <v>35.374025000000003</v>
@@ -5108,10 +5128,10 @@
         <v>103.84546330000001</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -5131,16 +5151,16 @@
         <v>204</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G41" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="J41">
         <v>35.031492499999999</v>
@@ -5149,10 +5169,10 @@
         <v>110.9389098</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -5172,16 +5192,16 @@
         <v>209</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="J42">
         <v>35.596111200000003</v>
@@ -5190,10 +5210,10 @@
         <v>116.9888847</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -5213,16 +5233,16 @@
         <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>365</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="J43">
         <v>37.426132299999999</v>
@@ -5231,10 +5251,10 @@
         <v>111.7808915</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -5254,16 +5274,16 @@
         <v>219</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="J44">
         <v>33.948200999999997</v>
@@ -5272,10 +5292,10 @@
         <v>118.2228186</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -5295,16 +5315,16 @@
         <v>224</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="J45">
         <v>23.113627999999999</v>
@@ -5313,10 +5333,10 @@
         <v>113.2447878</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -5336,16 +5356,16 @@
         <v>229</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>365</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="J46">
         <v>38.179308399999996</v>
@@ -5354,10 +5374,10 @@
         <v>112.4008678</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -5377,16 +5397,16 @@
         <v>234</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="I47" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="J47">
         <v>45.404457600000001</v>
@@ -5395,10 +5415,10 @@
         <v>12.2416616</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -5418,16 +5438,16 @@
         <v>239</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>365</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="J48">
         <v>42.804253899999999</v>
@@ -5436,13 +5456,13 @@
         <v>75.196181499999994</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N48" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -5462,16 +5482,16 @@
         <v>244</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>426</v>
-      </c>
       <c r="I49" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J49">
         <v>34.825284099999998</v>
@@ -5480,10 +5500,10 @@
         <v>133.55988909999999</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -5503,16 +5523,16 @@
         <v>249</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="J50">
         <v>34.307778800000001</v>
@@ -5521,10 +5541,10 @@
         <v>115.1838293</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -5544,16 +5564,16 @@
         <v>254</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="J51">
         <v>33.864195000000002</v>
@@ -5562,10 +5582,10 @@
         <v>115.78360929999999</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -5585,16 +5605,16 @@
         <v>259</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="J52">
         <v>38.1703993</v>
@@ -5603,10 +5623,10 @@
         <v>114.8879094</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -5626,16 +5646,16 @@
         <v>264</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="J53">
         <v>33.864195000000002</v>
@@ -5644,10 +5664,10 @@
         <v>115.78360929999999</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -5667,16 +5687,16 @@
         <v>269</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="J54">
         <v>31.259476100000001</v>
@@ -5685,10 +5705,10 @@
         <v>117.0239076</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -5708,16 +5728,16 @@
         <v>274</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J55">
         <v>40.6372249</v>
@@ -5726,10 +5746,10 @@
         <v>109.6417039</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -5749,16 +5769,16 @@
         <v>279</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="J56">
         <v>34.3395589</v>
@@ -5767,10 +5787,10 @@
         <v>108.63899069999999</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -5790,16 +5810,16 @@
         <v>284</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="J57">
         <v>34.2686493</v>
@@ -5808,10 +5828,10 @@
         <v>107.83880670000001</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -5831,16 +5851,16 @@
         <v>289</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G58" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="J58">
         <v>38.750803500000004</v>
@@ -5849,10 +5869,10 @@
         <v>116.049836</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -5872,16 +5892,16 @@
         <v>294</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="J59">
         <v>35.839595000000003</v>
@@ -5890,10 +5910,10 @@
         <v>115.7844053</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -5913,16 +5933,16 @@
         <v>299</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="J60">
         <v>35.973823500000002</v>
@@ -5931,10 +5951,10 @@
         <v>116.2166884</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -5954,28 +5974,28 @@
         <v>304</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>573</v>
+        <v>586</v>
       </c>
       <c r="J61">
-        <v>39.479145099999997</v>
+        <v>39.276691</v>
       </c>
       <c r="K61">
-        <v>115.85593780000001</v>
+        <v>115.4940443</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -5995,16 +6015,16 @@
         <v>309</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J62">
         <v>39.283397100000002</v>
@@ -6013,10 +6033,10 @@
         <v>115.64729920000001</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -6036,16 +6056,16 @@
         <v>314</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J63">
         <v>30.658453399999999</v>
@@ -6054,10 +6074,10 @@
         <v>103.935464</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -6077,16 +6097,16 @@
         <v>319</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J64">
         <v>34.413000500000003</v>
@@ -6095,10 +6115,10 @@
         <v>115.5775436</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -6118,16 +6138,16 @@
         <v>324</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G65" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="J65">
         <v>35.596111200000003</v>
@@ -6136,10 +6156,10 @@
         <v>116.9888847</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -6159,16 +6179,16 @@
         <v>329</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="J66">
         <v>29.970621000000001</v>
@@ -6177,10 +6197,10 @@
         <v>119.65154630000001</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -6200,16 +6220,16 @@
         <v>334</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J67">
         <v>34.384971899999996</v>
@@ -6218,10 +6238,10 @@
         <v>109.2722514</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -6241,16 +6261,16 @@
         <v>339</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J68">
         <v>35.092914999999998</v>
@@ -6259,10 +6279,10 @@
         <v>113.524289</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -6282,16 +6302,16 @@
         <v>344</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="J69">
         <v>34.413000500000003</v>
@@ -6300,10 +6320,10 @@
         <v>115.5775436</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -6323,16 +6343,16 @@
         <v>349</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="J70">
         <v>38.230331700000001</v>
@@ -6341,10 +6361,10 @@
         <v>114.4905485</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -6364,16 +6384,16 @@
         <v>354</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="J71">
         <v>30.764525200000001</v>
@@ -6382,10 +6402,10 @@
         <v>116.2269744</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -6405,16 +6425,16 @@
         <v>359</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="J72">
         <v>38.311072199999998</v>
@@ -6423,10 +6443,10 @@
         <v>115.0213562</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>